<commit_message>
wk4 xl files update
</commit_message>
<xml_diff>
--- a/static/output/Excel/LRcounts1-sol.xlsx
+++ b/static/output/Excel/LRcounts1-sol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bavanzi/Dropbox/My Mac (3160L-201016-M)/Documents/GitHub/ACTL20004-ACTL90021-Tutorials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adolphus\Documents\GitHub\ACTL20004-ACTL90021-Tutorials\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937E24E1-A163-C347-A3D0-8097FFF6079A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CA3BC8-2D71-4813-A6AD-926434CAC0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17260" yWindow="500" windowWidth="18580" windowHeight="20280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
     <sheet name="Chain Ladder" sheetId="6" r:id="rId6"/>
     <sheet name="Chain Ladder based IBNR" sheetId="8" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -523,7 +520,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -541,7 +538,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1265,7 +1262,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1881,7 +1878,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2605,7 +2602,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3221,7 +3218,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6825,117 +6822,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Data"/>
-      <sheetName val="Exposure based"/>
-      <sheetName val="Exposure based IBNR"/>
-      <sheetName val="Normaliser"/>
-      <sheetName val="Normaliser based IBNR"/>
-      <sheetName val="Chain Ladder"/>
-      <sheetName val="Chain Ladder based IBNR"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="4">
-          <cell r="A4">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>15</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -7229,9 +7115,9 @@
       <selection activeCell="B12" sqref="B12:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2148</v>
       </c>
@@ -7284,7 +7170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2064</v>
       </c>
@@ -7337,7 +7223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1996</v>
       </c>
@@ -7390,7 +7276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2131</v>
       </c>
@@ -7443,7 +7329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2033</v>
       </c>
@@ -7496,7 +7382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2144</v>
       </c>
@@ -7549,7 +7435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2073</v>
       </c>
@@ -7602,7 +7488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1958</v>
       </c>
@@ -7655,7 +7541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2137</v>
       </c>
@@ -7708,7 +7594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1858</v>
       </c>
@@ -7761,7 +7647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2076</v>
       </c>
@@ -7814,7 +7700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2027</v>
       </c>
@@ -7867,7 +7753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -7920,7 +7806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2014</v>
       </c>
@@ -7973,7 +7859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1809</v>
       </c>
@@ -8026,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1879</v>
       </c>
@@ -8088,16 +7974,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21E9C8B-005F-0D48-956E-E197840B02AB}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="18" width="6.6640625" customWidth="1"/>
+    <col min="3" max="18" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8119,7 +8005,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -8178,7 +8064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -8194,7 +8080,7 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0</v>
       </c>
@@ -8267,7 +8153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -8337,7 +8223,7 @@
       </c>
       <c r="R5" s="9"/>
     </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -8404,7 +8290,7 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
     </row>
-    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>3</v>
       </c>
@@ -8468,7 +8354,7 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>4</v>
       </c>
@@ -8529,7 +8415,7 @@
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
     </row>
-    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>5</v>
       </c>
@@ -8587,7 +8473,7 @@
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>6</v>
       </c>
@@ -8642,7 +8528,7 @@
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
     </row>
-    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>7</v>
       </c>
@@ -8694,7 +8580,7 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
     </row>
-    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>8</v>
       </c>
@@ -8743,7 +8629,7 @@
       <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
     </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>9</v>
       </c>
@@ -8789,7 +8675,7 @@
       <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
     </row>
-    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>10</v>
       </c>
@@ -8832,7 +8718,7 @@
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
     </row>
-    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>11</v>
       </c>
@@ -8872,7 +8758,7 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
     </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>12</v>
       </c>
@@ -8909,7 +8795,7 @@
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
     </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>13</v>
       </c>
@@ -8943,7 +8829,7 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>14</v>
       </c>
@@ -8974,7 +8860,7 @@
       <c r="Q18" s="9"/>
       <c r="R18" s="9"/>
     </row>
-    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>15</v>
       </c>
@@ -9002,7 +8888,7 @@
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
     </row>
-    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -9017,7 +8903,7 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -9037,7 +8923,7 @@
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
     </row>
-    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -9054,7 +8940,7 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -9069,7 +8955,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
@@ -9139,7 +9025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -9154,7 +9040,7 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>8</v>
       </c>
@@ -9209,7 +9095,7 @@
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
     </row>
-    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -9224,7 +9110,7 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>9</v>
       </c>
@@ -9286,7 +9172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -9302,7 +9188,7 @@
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -9318,7 +9204,7 @@
       <c r="M30" s="10"/>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>10</v>
       </c>
@@ -9388,7 +9274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>11</v>
       </c>
@@ -9406,7 +9292,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
     </row>
-    <row r="33" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -9422,7 +9308,7 @@
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
     </row>
-    <row r="34" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>10</v>
       </c>
@@ -9483,7 +9369,7 @@
       <c r="Q34" s="9"/>
       <c r="R34" s="9"/>
     </row>
-    <row r="35" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>12</v>
       </c>
@@ -9501,7 +9387,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
     </row>
-    <row r="36" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -9517,7 +9403,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
     </row>
-    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -9533,7 +9419,7 @@
       <c r="M37" s="10"/>
       <c r="N37" s="6"/>
     </row>
-    <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>13</v>
       </c>
@@ -9551,7 +9437,7 @@
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
     </row>
-    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -9568,7 +9454,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
     </row>
-    <row r="40" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>15</v>
       </c>
@@ -9598,7 +9484,7 @@
       </c>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -9616,7 +9502,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
     </row>
-    <row r="42" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>17</v>
       </c>
@@ -9654,7 +9540,7 @@
         <v>-2.7622278611067426</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>19</v>
       </c>
@@ -9692,7 +9578,7 @@
         <v>6.3150920044034262E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -9708,7 +9594,7 @@
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
     </row>
-    <row r="45" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>54</v>
       </c>
@@ -9726,7 +9612,7 @@
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
     </row>
-    <row r="46" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>22</v>
       </c>
@@ -9747,7 +9633,7 @@
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
     </row>
-    <row r="47" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>23</v>
       </c>
@@ -9768,7 +9654,7 @@
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
     </row>
-    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>55</v>
       </c>
@@ -9789,7 +9675,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
     </row>
-    <row r="49" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -9819,13 +9705,13 @@
       <selection activeCell="C25" sqref="C25:O40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="14" width="6.5" customWidth="1"/>
-    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="6.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -9852,7 +9738,7 @@
       </c>
       <c r="S1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -9914,7 +9800,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="6"/>
@@ -9935,7 +9821,7 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
     </row>
-    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>'Exposure based'!A4</f>
         <v>0</v>
@@ -10017,7 +9903,7 @@
         <v>9.2687091725423415E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>'Exposure based'!A5</f>
         <v>1</v>
@@ -10099,7 +9985,7 @@
         <v>0.10178695747398346</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>'Exposure based'!A6</f>
         <v>2</v>
@@ -10181,7 +10067,7 @@
         <v>9.1225136156930745E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <f>'Exposure based'!A7</f>
         <v>3</v>
@@ -10263,7 +10149,7 @@
         <v>0.11031963674891716</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <f>'Exposure based'!A8</f>
         <v>4</v>
@@ -10345,7 +10231,7 @@
         <v>0.10137085799904094</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f>'Exposure based'!A9</f>
         <v>5</v>
@@ -10427,7 +10313,7 @@
         <v>9.1523832795277052E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f>'Exposure based'!A10</f>
         <v>6</v>
@@ -10509,7 +10395,7 @@
         <v>9.5293669511178208E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <f>'Exposure based'!A11</f>
         <v>7</v>
@@ -10591,7 +10477,7 @@
         <v>9.7176682326977556E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <f>'Exposure based'!A12</f>
         <v>8</v>
@@ -10673,7 +10559,7 @@
         <v>8.4435144341872617E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <f>'Exposure based'!A13</f>
         <v>9</v>
@@ -10755,7 +10641,7 @@
         <v>0.10498721201735624</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <f>'Exposure based'!A14</f>
         <v>10</v>
@@ -10837,7 +10723,7 @@
         <v>9.5220154450587555E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <f>'Exposure based'!A15</f>
         <v>11</v>
@@ -10919,7 +10805,7 @@
         <v>9.4716487164467442E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <f>'Exposure based'!A16</f>
         <v>12</v>
@@ -11001,7 +10887,7 @@
         <v>9.8398261601542525E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <f>'Exposure based'!A17</f>
         <v>13</v>
@@ -11083,7 +10969,7 @@
         <v>9.1356847238587904E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <f>'Exposure based'!A18</f>
         <v>14</v>
@@ -11165,7 +11051,7 @@
         <v>9.5492518951464725E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <f>'Exposure based'!A19</f>
         <v>15</v>
@@ -11247,7 +11133,7 @@
         <v>9.75599886655662E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -11268,7 +11154,7 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
     </row>
-    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -11292,8 +11178,8 @@
       </c>
       <c r="S21" s="3"/>
     </row>
-    <row r="22" spans="1:20" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -11310,7 +11196,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C25" s="25">
         <v>4</v>
       </c>
@@ -11371,7 +11257,7 @@
         <v>0.9995385395455223</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C26" s="25">
         <v>3</v>
       </c>
@@ -11432,7 +11318,7 @@
         <v>0.99957979461678315</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C27" s="25">
         <v>4</v>
       </c>
@@ -11493,7 +11379,7 @@
         <v>0.9995311442736764</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C28" s="25">
         <v>4</v>
       </c>
@@ -11554,7 +11440,7 @@
         <v>0.99961229542869889</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C29" s="25">
         <v>4</v>
       </c>
@@ -11615,7 +11501,7 @@
         <v>0.99957806978932506</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C30" s="25">
         <v>2</v>
       </c>
@@ -11676,7 +11562,7 @@
         <v>0.99884268016011979</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C31" s="25">
         <v>1</v>
       </c>
@@ -11737,7 +11623,7 @@
         <v>0.9972473094054648</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C32" s="25">
         <v>3</v>
       </c>
@@ -11798,7 +11684,7 @@
         <v>1.0195933038023302</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C33" s="25">
         <v>1</v>
       </c>
@@ -11859,7 +11745,7 @@
         <v>0.99203103432804052</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C34" s="25">
         <v>2</v>
       </c>
@@ -11920,7 +11806,7 @@
         <v>1.0047868871215009</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="25">
         <v>3</v>
       </c>
@@ -11981,7 +11867,7 @@
         <v>1.0218687984532593</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="25">
         <v>6</v>
       </c>
@@ -12042,7 +11928,7 @@
         <v>1.0052590178522891</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C37" s="25">
         <v>4</v>
       </c>
@@ -12103,7 +11989,7 @@
         <v>1.0586230383671098</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C38" s="25">
         <v>0</v>
       </c>
@@ -12164,7 +12050,7 @@
         <v>1.0380847176515093</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C39" s="25">
         <v>1</v>
       </c>
@@ -12225,7 +12111,7 @@
         <v>0.92042669916310571</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C40" s="25">
         <v>5</v>
       </c>
@@ -12286,13 +12172,13 @@
         <v>1.0146457087218534</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="P41" s="6"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="26"/>
       <c r="S41" s="3"/>
     </row>
-    <row r="42" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>38</v>
       </c>
@@ -12314,37 +12200,37 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="O43">
         <f t="shared" ref="O43" si="8">IF(O4&gt;0,O25/O4,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="O44">
         <f t="shared" ref="O44" si="9">IF(O5&gt;0,O26/O5,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="O45">
         <f t="shared" ref="O45:O46" si="10">IF(O6&gt;0,O27/O6,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="O46">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="O47">
         <f t="shared" ref="O47" si="11">IF(O8&gt;0,O29/O8,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M48" t="str">
         <f t="shared" ref="M48:O48" si="12">IF(M9&gt;0,M30/M9,"")</f>
         <v/>
@@ -12358,7 +12244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L49">
         <f t="shared" ref="L49:O49" si="13">IF(L10&gt;0,L31/L10,"")</f>
         <v>1</v>
@@ -12376,7 +12262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
       <c r="K50">
         <f t="shared" ref="K50:O50" si="14">IF(K11&gt;0,K32/K11,"")</f>
         <v>1</v>
@@ -12398,7 +12284,7 @@
         <v>11.940803943538015</v>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J51">
         <f t="shared" ref="J51:O51" si="15">IF(J12&gt;0,J33/J12,"")</f>
         <v>1</v>
@@ -12424,7 +12310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I52">
         <f t="shared" ref="I52:O52" si="16">IF(I13&gt;0,I34/I13,"")</f>
         <v>1</v>
@@ -12454,7 +12340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H53">
         <f t="shared" ref="H53:O53" si="17">IF(H14&gt;0,H35/H14,"")</f>
         <v>1</v>
@@ -12488,7 +12374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
       <c r="G54">
         <f t="shared" ref="G54:O54" si="18">IF(G15&gt;0,G36/G15,"")</f>
         <v>1</v>
@@ -12526,7 +12412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F55">
         <f t="shared" ref="F55:O55" si="19">IF(F16&gt;0,F37/F16,"")</f>
         <v>1</v>
@@ -12568,7 +12454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E56">
         <f t="shared" ref="E56:O56" si="20">IF(E17&gt;0,E38/E17,"")</f>
         <v>1</v>
@@ -12614,7 +12500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D57">
         <f t="shared" ref="D57:O57" si="21">IF(D18&gt;0,D39/D18,"")</f>
         <v>1</v>
@@ -12664,7 +12550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C58">
         <f t="shared" ref="C58:O58" si="22">IF(C19&gt;0,C40/C19,"")</f>
         <v>1</v>
@@ -12718,7 +12604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C59" t="str">
         <f t="shared" ref="C59:O59" si="23">IF(C41&gt;0,C20/C41,"")</f>
         <v/>
@@ -12772,7 +12658,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C60" t="str">
         <f t="shared" ref="C60:O60" si="24">IF(C42&gt;0,C21/C42,"")</f>
         <v/>
@@ -12852,12 +12738,12 @@
       <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="18" width="7.6640625" customWidth="1"/>
+    <col min="3" max="18" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12879,7 +12765,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -12938,7 +12824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -12954,7 +12840,7 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0</v>
       </c>
@@ -13027,7 +12913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -13097,7 +12983,7 @@
       </c>
       <c r="R5" s="9"/>
     </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -13164,7 +13050,7 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
     </row>
-    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>3</v>
       </c>
@@ -13228,7 +13114,7 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>4</v>
       </c>
@@ -13289,7 +13175,7 @@
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
     </row>
-    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>5</v>
       </c>
@@ -13347,7 +13233,7 @@
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>6</v>
       </c>
@@ -13402,7 +13288,7 @@
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
     </row>
-    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>7</v>
       </c>
@@ -13454,7 +13340,7 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
     </row>
-    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>8</v>
       </c>
@@ -13503,7 +13389,7 @@
       <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
     </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>9</v>
       </c>
@@ -13549,7 +13435,7 @@
       <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
     </row>
-    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>10</v>
       </c>
@@ -13592,7 +13478,7 @@
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
     </row>
-    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>11</v>
       </c>
@@ -13632,7 +13518,7 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
     </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>12</v>
       </c>
@@ -13669,7 +13555,7 @@
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
     </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>13</v>
       </c>
@@ -13703,7 +13589,7 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>14</v>
       </c>
@@ -13734,7 +13620,7 @@
       <c r="Q18" s="9"/>
       <c r="R18" s="9"/>
     </row>
-    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
@@ -13754,7 +13640,7 @@
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
     </row>
-    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -13769,7 +13655,7 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -13789,7 +13675,7 @@
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
     </row>
-    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -13806,7 +13692,7 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -13821,7 +13707,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
@@ -13891,7 +13777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -13906,7 +13792,7 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>8</v>
       </c>
@@ -13961,7 +13847,7 @@
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
     </row>
-    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -13976,7 +13862,7 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>9</v>
       </c>
@@ -14038,7 +13924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="52" t="s">
@@ -14056,7 +13942,7 @@
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -14072,7 +13958,7 @@
       <c r="M30" s="10"/>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>10</v>
       </c>
@@ -14142,7 +14028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>11</v>
       </c>
@@ -14160,7 +14046,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
     </row>
-    <row r="33" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -14176,7 +14062,7 @@
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
     </row>
-    <row r="34" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>10</v>
       </c>
@@ -14237,7 +14123,7 @@
       <c r="Q34" s="9"/>
       <c r="R34" s="9"/>
     </row>
-    <row r="35" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>12</v>
       </c>
@@ -14255,7 +14141,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
     </row>
-    <row r="36" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -14271,7 +14157,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
     </row>
-    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -14287,7 +14173,7 @@
       <c r="M37" s="10"/>
       <c r="N37" s="6"/>
     </row>
-    <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>13</v>
       </c>
@@ -14305,7 +14191,7 @@
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
     </row>
-    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -14322,7 +14208,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
     </row>
-    <row r="40" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>15</v>
       </c>
@@ -14352,7 +14238,7 @@
       </c>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -14370,7 +14256,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
     </row>
-    <row r="42" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>17</v>
       </c>
@@ -14408,7 +14294,7 @@
         <v>1.2631163087176125</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>19</v>
       </c>
@@ -14446,7 +14332,7 @@
         <v>3.5364249252295079</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -14462,7 +14348,7 @@
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
     </row>
-    <row r="45" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>21</v>
       </c>
@@ -14480,7 +14366,7 @@
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
     </row>
-    <row r="46" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>22</v>
       </c>
@@ -14501,7 +14387,7 @@
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
     </row>
-    <row r="47" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>23</v>
       </c>
@@ -14522,7 +14408,7 @@
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
     </row>
-    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>24</v>
       </c>
@@ -14543,7 +14429,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
     </row>
-    <row r="49" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -14573,13 +14459,13 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="14" width="6.5" customWidth="1"/>
-    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="6.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -14606,7 +14492,7 @@
       </c>
       <c r="S1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -14668,7 +14554,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="6"/>
@@ -14689,9 +14575,8 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
     </row>
-    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
-        <f>'[1]Exposure based'!A4</f>
         <v>0</v>
       </c>
       <c r="B4" s="23">
@@ -14771,9 +14656,8 @@
         <v>9.2690979700957465E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <f>'[1]Exposure based'!A5</f>
         <v>1</v>
       </c>
       <c r="B5" s="23">
@@ -14853,9 +14737,8 @@
         <v>0.10179177321206564</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
-        <f>'[1]Exposure based'!A6</f>
         <v>2</v>
       </c>
       <c r="B6" s="23">
@@ -14935,9 +14818,8 @@
         <v>9.1219522071275497E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
-        <f>'[1]Exposure based'!A7</f>
         <v>3</v>
       </c>
       <c r="B7" s="23">
@@ -15017,9 +14899,8 @@
         <v>0.1103144906232404</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <f>'[1]Exposure based'!A8</f>
         <v>4</v>
       </c>
       <c r="B8" s="23">
@@ -15099,9 +14980,8 @@
         <v>0.10137146948841015</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <f>'[1]Exposure based'!A9</f>
         <v>5</v>
       </c>
       <c r="B9" s="23">
@@ -15181,9 +15061,8 @@
         <v>9.1500610639975555E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <f>'[1]Exposure based'!A10</f>
         <v>6</v>
       </c>
       <c r="B10" s="23">
@@ -15263,9 +15142,8 @@
         <v>9.5230846683027587E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
-        <f>'[1]Exposure based'!A11</f>
         <v>7</v>
       </c>
       <c r="B11" s="23">
@@ -15345,9 +15223,8 @@
         <v>9.7327134963581086E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <f>'[1]Exposure based'!A12</f>
         <v>8</v>
       </c>
       <c r="B12" s="23">
@@ -15427,9 +15304,8 @@
         <v>8.5017029065906635E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
-        <f>'[1]Exposure based'!A13</f>
         <v>9</v>
       </c>
       <c r="B13" s="23">
@@ -15509,9 +15385,8 @@
         <v>0.10836659754707068</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
-        <f>'[1]Exposure based'!A14</f>
         <v>10</v>
       </c>
       <c r="B14" s="23">
@@ -15591,9 +15466,8 @@
         <v>9.7129283427356869E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
-        <f>'[1]Exposure based'!A15</f>
         <v>11</v>
       </c>
       <c r="B15" s="23">
@@ -15673,9 +15547,8 @@
         <v>8.9990887171243122E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <f>'[1]Exposure based'!A16</f>
         <v>12</v>
       </c>
       <c r="B16" s="23">
@@ -15755,9 +15628,8 @@
         <v>9.5783992032493284E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <f>'[1]Exposure based'!A17</f>
         <v>13</v>
       </c>
       <c r="B17" s="23">
@@ -15837,9 +15709,8 @@
         <v>8.5241397753733697E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
-        <f>'[1]Exposure based'!A18</f>
         <v>14</v>
       </c>
       <c r="B18" s="23">
@@ -15919,9 +15790,8 @@
         <v>9.5081162086530016E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
-        <f>'[1]Exposure based'!A19</f>
         <v>15</v>
       </c>
       <c r="B19" s="23"/>
@@ -15998,7 +15868,7 @@
         <v>0.2912605243363805</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -16019,7 +15889,7 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
     </row>
-    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -16043,8 +15913,8 @@
       </c>
       <c r="S21" s="3"/>
     </row>
-    <row r="22" spans="1:20" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -16061,7 +15931,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C25" s="25">
         <v>4</v>
       </c>
@@ -16122,7 +15992,7 @@
         <v>0.99949661333652517</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C26" s="25">
         <v>3</v>
       </c>
@@ -16183,7 +16053,7 @@
         <v>0.9995325047982524</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C27" s="25">
         <v>4</v>
       </c>
@@ -16244,7 +16114,7 @@
         <v>0.99959266020065807</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C28" s="25">
         <v>4</v>
       </c>
@@ -16305,7 +16175,7 @@
         <v>0.99965892693169767</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C29" s="25">
         <v>4</v>
       </c>
@@ -16366,7 +16236,7 @@
         <v>0.99957204017007961</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C30" s="25">
         <v>2</v>
       </c>
@@ -16427,7 +16297,7 @@
         <v>0.99909617879448087</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C31" s="25">
         <v>1</v>
       </c>
@@ -16488,7 +16358,7 @@
         <v>0.99790518338773626</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C32" s="25">
         <v>3</v>
       </c>
@@ -16549,7 +16419,7 @@
         <v>1.0180171708885466</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C33" s="25">
         <v>1</v>
       </c>
@@ -16610,7 +16480,7 @@
         <v>0.98524124514126865</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C34" s="25">
         <v>2</v>
       </c>
@@ -16671,7 +16541,7 @@
         <v>0.97345285667627701</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="25">
         <v>3</v>
       </c>
@@ -16732,7 +16602,7 @@
         <v>1.0017834105584478</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="25">
         <v>6</v>
       </c>
@@ -16793,7 +16663,7 @@
         <v>1.0580471629331554</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C37" s="25">
         <v>4</v>
       </c>
@@ -16854,7 +16724,7 @@
         <v>1.087516446707814</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C38" s="25">
         <v>0</v>
       </c>
@@ -16921,7 +16791,7 @@
       <c r="W38" s="50"/>
       <c r="X38" s="50"/>
     </row>
-    <row r="39" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C39" s="25">
         <v>1</v>
       </c>
@@ -16988,7 +16858,7 @@
       <c r="W39" s="50"/>
       <c r="X39" s="50"/>
     </row>
-    <row r="40" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C40" s="25">
         <v>5</v>
       </c>
@@ -17055,13 +16925,13 @@
       <c r="W40" s="50"/>
       <c r="X40" s="50"/>
     </row>
-    <row r="41" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="P41" s="6"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="26"/>
       <c r="S41" s="3"/>
     </row>
-    <row r="42" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>38</v>
       </c>
@@ -17083,37 +16953,37 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O43">
         <f t="shared" ref="O43:O47" si="6">IF(O4&gt;0,O25/O4,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O44">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O45">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O47">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M48" t="str">
         <f t="shared" ref="M48:O48" si="7">IF(M9&gt;0,M30/M9,"")</f>
         <v/>
@@ -17127,7 +16997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L49">
         <f t="shared" ref="L49:O49" si="8">IF(L10&gt;0,L31/L10,"")</f>
         <v>1</v>
@@ -17145,7 +17015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
       <c r="K50">
         <f t="shared" ref="K50:O50" si="9">IF(K11&gt;0,K32/K11,"")</f>
         <v>1</v>
@@ -17167,7 +17037,7 @@
         <v>13.483257399871126</v>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J51">
         <f t="shared" ref="J51:O51" si="10">IF(J12&gt;0,J33/J12,"")</f>
         <v>1</v>
@@ -17193,7 +17063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I52">
         <f t="shared" ref="I52:O52" si="11">IF(I13&gt;0,I34/I13,"")</f>
         <v>1</v>
@@ -17223,7 +17093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H53">
         <f t="shared" ref="H53:O53" si="12">IF(H14&gt;0,H35/H14,"")</f>
         <v>1</v>
@@ -17257,7 +17127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
       <c r="G54">
         <f t="shared" ref="G54:O54" si="13">IF(G15&gt;0,G36/G15,"")</f>
         <v>1</v>
@@ -17295,7 +17165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F55">
         <f t="shared" ref="F55:O55" si="14">IF(F16&gt;0,F37/F16,"")</f>
         <v>1</v>
@@ -17337,7 +17207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E56">
         <f t="shared" ref="E56:O56" si="15">IF(E17&gt;0,E38/E17,"")</f>
         <v>1</v>
@@ -17383,7 +17253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D57">
         <f t="shared" ref="D57:O57" si="16">IF(D18&gt;0,D39/D18,"")</f>
         <v>1</v>
@@ -17433,7 +17303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C58">
         <f t="shared" ref="C58:O58" si="17">IF(C19&gt;0,C40/C19,"")</f>
         <v>1</v>
@@ -17487,7 +17357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C59" t="str">
         <f t="shared" ref="C59:O60" si="18">IF(C41&gt;0,C20/C41,"")</f>
         <v/>
@@ -17541,7 +17411,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C60" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17621,12 +17491,12 @@
       <selection activeCell="C29" sqref="C29:F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="18" width="9.1640625" customWidth="1"/>
+    <col min="3" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17646,7 +17516,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -17700,7 +17570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -17716,7 +17586,7 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0</v>
       </c>
@@ -17783,7 +17653,7 @@
       </c>
       <c r="R4" s="9"/>
     </row>
-    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -17847,7 +17717,7 @@
       <c r="Q5" s="31"/>
       <c r="R5" s="9"/>
     </row>
-    <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -17908,7 +17778,7 @@
       <c r="Q6" s="31"/>
       <c r="R6" s="9"/>
     </row>
-    <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>3</v>
       </c>
@@ -17966,7 +17836,7 @@
       <c r="Q7" s="31"/>
       <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>4</v>
       </c>
@@ -18021,7 +17891,7 @@
       <c r="Q8" s="31"/>
       <c r="R8" s="9"/>
     </row>
-    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>5</v>
       </c>
@@ -18073,7 +17943,7 @@
       <c r="Q9" s="31"/>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>6</v>
       </c>
@@ -18122,7 +17992,7 @@
       <c r="Q10" s="31"/>
       <c r="R10" s="9"/>
     </row>
-    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>7</v>
       </c>
@@ -18168,7 +18038,7 @@
       <c r="Q11" s="31"/>
       <c r="R11" s="9"/>
     </row>
-    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>8</v>
       </c>
@@ -18211,7 +18081,7 @@
       <c r="Q12" s="31"/>
       <c r="R12" s="9"/>
     </row>
-    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>9</v>
       </c>
@@ -18251,7 +18121,7 @@
       <c r="Q13" s="31"/>
       <c r="R13" s="9"/>
     </row>
-    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>10</v>
       </c>
@@ -18288,7 +18158,7 @@
       <c r="Q14" s="31"/>
       <c r="R14" s="9"/>
     </row>
-    <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>11</v>
       </c>
@@ -18322,7 +18192,7 @@
       <c r="Q15" s="31"/>
       <c r="R15" s="9"/>
     </row>
-    <row r="16" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>12</v>
       </c>
@@ -18353,7 +18223,7 @@
       <c r="Q16" s="31"/>
       <c r="R16" s="9"/>
     </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>13</v>
       </c>
@@ -18378,7 +18248,7 @@
       <c r="Q17" s="31"/>
       <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>14</v>
       </c>
@@ -18403,7 +18273,7 @@
       <c r="Q18" s="31"/>
       <c r="R18" s="9"/>
     </row>
-    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>15</v>
       </c>
@@ -18425,7 +18295,7 @@
       <c r="Q19" s="31"/>
       <c r="R19" s="9"/>
     </row>
-    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -18440,7 +18310,7 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -18460,7 +18330,7 @@
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
     </row>
-    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -18477,7 +18347,7 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -18492,7 +18362,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
@@ -18559,7 +18429,7 @@
       </c>
       <c r="R24" s="33"/>
     </row>
-    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="34"/>
@@ -18579,7 +18449,7 @@
       <c r="Q25" s="35"/>
       <c r="R25" s="35"/>
     </row>
-    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>8</v>
       </c>
@@ -18631,7 +18501,7 @@
       <c r="Q26" s="34"/>
       <c r="R26" s="34"/>
     </row>
-    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="34"/>
@@ -18651,7 +18521,7 @@
       <c r="Q27" s="35"/>
       <c r="R27" s="35"/>
     </row>
-    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>9</v>
       </c>
@@ -18712,7 +18582,7 @@
       <c r="Q28" s="35"/>
       <c r="R28" s="35"/>
     </row>
-    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="56" t="s">
@@ -18734,7 +18604,7 @@
       <c r="Q29" s="35"/>
       <c r="R29" s="35"/>
     </row>
-    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="38"/>
@@ -18754,7 +18624,7 @@
       <c r="Q30" s="35"/>
       <c r="R30" s="35"/>
     </row>
-    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>10</v>
       </c>
@@ -18824,12 +18694,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="39" t="s">
         <v>10</v>
       </c>
@@ -18881,7 +18751,7 @@
       <c r="N34" s="43"/>
       <c r="O34" s="43"/>
     </row>
-    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="39" t="s">
         <v>12</v>
       </c>
@@ -18900,7 +18770,7 @@
       <c r="N35" s="7"/>
       <c r="O35" s="44"/>
     </row>
-    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -18917,7 +18787,7 @@
       <c r="N36" s="7"/>
       <c r="O36" s="44"/>
     </row>
-    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="45"/>
       <c r="B37" s="45"/>
       <c r="C37" s="45"/>
@@ -18934,7 +18804,7 @@
       <c r="N37" s="7"/>
       <c r="O37" s="44"/>
     </row>
-    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="39" t="s">
         <v>13</v>
       </c>
@@ -18953,7 +18823,7 @@
       <c r="N38" s="7"/>
       <c r="O38" s="44"/>
     </row>
-    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -18972,7 +18842,7 @@
       <c r="N39" s="7"/>
       <c r="O39" s="44"/>
     </row>
-    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>15</v>
       </c>
@@ -19006,7 +18876,7 @@
       <c r="N40" s="7"/>
       <c r="O40" s="44"/>
     </row>
-    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -19025,7 +18895,7 @@
       <c r="N41" s="7"/>
       <c r="O41" s="44"/>
     </row>
-    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>17</v>
       </c>
@@ -19067,7 +18937,7 @@
       <c r="N42" s="7"/>
       <c r="O42" s="44"/>
     </row>
-    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>19</v>
       </c>
@@ -19109,7 +18979,7 @@
       <c r="N43" s="7"/>
       <c r="O43" s="44"/>
     </row>
-    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -19126,7 +18996,7 @@
       <c r="N44" s="7"/>
       <c r="O44" s="44"/>
     </row>
-    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -19143,7 +19013,7 @@
       <c r="N45" s="7"/>
       <c r="O45" s="44"/>
     </row>
-    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="39" t="s">
         <v>21</v>
       </c>
@@ -19162,7 +19032,7 @@
       <c r="N46" s="7"/>
       <c r="O46" s="44"/>
     </row>
-    <row r="47" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>22</v>
       </c>
@@ -19184,7 +19054,7 @@
       <c r="N47" s="7"/>
       <c r="O47" s="44"/>
     </row>
-    <row r="48" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>23</v>
       </c>
@@ -19206,7 +19076,7 @@
       <c r="N48" s="7"/>
       <c r="O48" s="44"/>
     </row>
-    <row r="49" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>41</v>
       </c>
@@ -19228,7 +19098,7 @@
       <c r="N49" s="7"/>
       <c r="O49" s="44"/>
     </row>
-    <row r="50" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>42</v>
       </c>
@@ -19252,7 +19122,7 @@
       <c r="N50" s="7"/>
       <c r="O50" s="44"/>
     </row>
-    <row r="51" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -19269,7 +19139,7 @@
       <c r="N51" s="7"/>
       <c r="O51" s="44"/>
     </row>
-    <row r="52" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="45"/>
       <c r="B52" s="45"/>
       <c r="C52" s="45"/>
@@ -19286,7 +19156,7 @@
       <c r="N52" s="45"/>
       <c r="O52" s="44"/>
     </row>
-    <row r="53" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="39" t="s">
         <v>44</v>
       </c>
@@ -19305,7 +19175,7 @@
       <c r="N53" s="7"/>
       <c r="O53" s="44"/>
     </row>
-    <row r="54" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="39">
@@ -19346,7 +19216,7 @@
       </c>
       <c r="O54" s="39"/>
     </row>
-    <row r="55" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>46</v>
       </c>
@@ -19400,7 +19270,7 @@
       </c>
       <c r="O55" s="44"/>
     </row>
-    <row r="56" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>47</v>
       </c>
@@ -19455,7 +19325,7 @@
       </c>
       <c r="O56" s="44"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C57" s="50" t="s">
         <v>48</v>
       </c>
@@ -19464,7 +19334,7 @@
       <c r="F57" s="50"/>
       <c r="G57" s="50"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C58" s="50" t="s">
         <v>49</v>
       </c>
@@ -19486,13 +19356,13 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="14" width="6.5" customWidth="1"/>
-    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="6.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -19519,7 +19389,7 @@
       </c>
       <c r="S1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -19577,7 +19447,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="6"/>
@@ -19598,9 +19468,8 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
     </row>
-    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
-        <f>'[1]Exposure based'!A4</f>
         <v>0</v>
       </c>
       <c r="B4" s="23"/>
@@ -19674,9 +19543,8 @@
         <v>9.2773186432174207E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <f>'[1]Exposure based'!A5</f>
         <v>1</v>
       </c>
       <c r="B5" s="23"/>
@@ -19750,9 +19618,8 @@
         <v>0.1018857098862168</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
-        <f>'[1]Exposure based'!A6</f>
         <v>2</v>
       </c>
       <c r="B6" s="23"/>
@@ -19826,9 +19693,8 @@
         <v>9.1309197316866028E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
-        <f>'[1]Exposure based'!A7</f>
         <v>3</v>
       </c>
       <c r="B7" s="23"/>
@@ -19902,9 +19768,8 @@
         <v>0.11043025792319858</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <f>'[1]Exposure based'!A8</f>
         <v>4</v>
       </c>
       <c r="B8" s="23"/>
@@ -19978,9 +19843,8 @@
         <v>0.10146903162640528</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <f>'[1]Exposure based'!A9</f>
         <v>5</v>
       </c>
       <c r="B9" s="23"/>
@@ -20054,9 +19918,8 @@
         <v>9.1545070673884343E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <f>'[1]Exposure based'!A10</f>
         <v>6</v>
       </c>
       <c r="B10" s="23"/>
@@ -20130,9 +19993,8 @@
         <v>9.5333038757032917E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
-        <f>'[1]Exposure based'!A11</f>
         <v>7</v>
       </c>
       <c r="B11" s="23"/>
@@ -20206,9 +20068,8 @@
         <v>9.7226815977718276E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <f>'[1]Exposure based'!A12</f>
         <v>8</v>
       </c>
       <c r="B12" s="23"/>
@@ -20282,9 +20143,8 @@
         <v>8.4199584336922553E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
-        <f>'[1]Exposure based'!A13</f>
         <v>9</v>
       </c>
       <c r="B13" s="23"/>
@@ -20358,9 +20218,8 @@
         <v>0.10503441610853555</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
-        <f>'[1]Exposure based'!A14</f>
         <v>10</v>
       </c>
       <c r="B14" s="23"/>
@@ -20434,9 +20293,8 @@
         <v>9.5388482165810334E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
-        <f>'[1]Exposure based'!A15</f>
         <v>11</v>
       </c>
       <c r="B15" s="23"/>
@@ -20510,9 +20368,8 @@
         <v>9.4632496893869669E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <f>'[1]Exposure based'!A16</f>
         <v>12</v>
       </c>
       <c r="B16" s="23"/>
@@ -20586,9 +20443,8 @@
         <v>9.9480483731164859E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <f>'[1]Exposure based'!A17</f>
         <v>13</v>
       </c>
       <c r="B17" s="23"/>
@@ -20662,9 +20518,8 @@
         <v>8.5772866606746892E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
-        <f>'[1]Exposure based'!A18</f>
         <v>14</v>
       </c>
       <c r="B18" s="23"/>
@@ -20738,9 +20593,8 @@
         <v>9.2035395092272834E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
-        <f>'[1]Exposure based'!A19</f>
         <v>15</v>
       </c>
       <c r="B19" s="23"/>
@@ -20814,7 +20668,7 @@
         <v>0.17420874179038018</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -20835,7 +20689,7 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
     </row>
-    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -20859,8 +20713,8 @@
       </c>
       <c r="S21" s="3"/>
     </row>
-    <row r="22" spans="1:20" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
@@ -20877,7 +20731,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C25" s="25">
         <v>4</v>
       </c>
@@ -20936,7 +20790,7 @@
         <v>0.9986109549625436</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C26" s="25">
         <v>3</v>
       </c>
@@ -20995,7 +20849,7 @@
         <v>0.9986109549625436</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C27" s="25">
         <v>4</v>
       </c>
@@ -21054,7 +20908,7 @@
         <v>0.99861095496254371</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C28" s="25">
         <v>4</v>
       </c>
@@ -21113,7 +20967,7 @@
         <v>0.9986109549625436</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C29" s="25">
         <v>4</v>
       </c>
@@ -21172,7 +21026,7 @@
         <v>0.9986109549625436</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C30" s="25">
         <v>2</v>
       </c>
@@ -21231,7 +21085,7 @@
         <v>0.99861095496254371</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C31" s="25">
         <v>1</v>
       </c>
@@ -21290,7 +21144,7 @@
         <v>0.99683548077801498</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C32" s="25">
         <v>3</v>
       </c>
@@ -21349,7 +21203,7 @@
         <v>1.0190675647448864</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C33" s="25">
         <v>1</v>
       </c>
@@ -21408,7 +21262,7 @@
         <v>0.99480637861503673</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C34" s="25">
         <v>2</v>
       </c>
@@ -21467,7 +21321,7 @@
         <v>1.004335320353267</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="25">
         <v>3</v>
       </c>
@@ -21526,7 +21380,7 @@
         <v>1.020065553069796</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="25">
         <v>6</v>
       </c>
@@ -21585,7 +21439,7 @@
         <v>1.0061512269739077</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C37" s="25">
         <v>4</v>
       </c>
@@ -21644,7 +21498,7 @@
         <v>1.0471065555749177</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C38" s="25">
         <v>0</v>
       </c>
@@ -21703,7 +21557,7 @@
         <v>1.1056660541148542</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C39" s="25">
         <v>1</v>
       </c>
@@ -21762,7 +21616,7 @@
         <v>0.95500067039584469</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C40" s="25">
         <v>5</v>
       </c>
@@ -21828,13 +21682,13 @@
       <c r="X40" s="50"/>
       <c r="Y40" s="50"/>
     </row>
-    <row r="41" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="P41" s="6"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="26"/>
       <c r="S41" s="3"/>
     </row>
-    <row r="42" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>38</v>
       </c>
@@ -21856,37 +21710,37 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="O43" t="str">
         <f t="shared" ref="O43:O47" si="6">IF(O4&gt;0,O25/O4,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="O44" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="O45" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="O46" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="O47" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="M48" t="str">
         <f t="shared" ref="M48:O48" si="7">IF(M9&gt;0,M30/M9,"")</f>
         <v/>
@@ -21900,7 +21754,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L49">
         <f t="shared" ref="L49:O49" si="8">IF(L10&gt;0,L31/L10,"")</f>
         <v>1</v>
@@ -21918,7 +21772,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
       <c r="K50">
         <f t="shared" ref="K50:O50" si="9">IF(K11&gt;0,K32/K11,"")</f>
         <v>1</v>
@@ -21940,7 +21794,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J51">
         <f t="shared" ref="J51:O51" si="10">IF(J12&gt;0,J33/J12,"")</f>
         <v>1</v>
@@ -21966,7 +21820,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="I52">
         <f t="shared" ref="I52:O52" si="11">IF(I13&gt;0,I34/I13,"")</f>
         <v>1</v>
@@ -21996,7 +21850,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H53">
         <f t="shared" ref="H53:O53" si="12">IF(H14&gt;0,H35/H14,"")</f>
         <v>1</v>
@@ -22030,7 +21884,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
       <c r="G54">
         <f t="shared" ref="G54:O54" si="13">IF(G15&gt;0,G36/G15,"")</f>
         <v>1</v>
@@ -22068,7 +21922,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F55">
         <f t="shared" ref="F55:O55" si="14">IF(F16&gt;0,F37/F16,"")</f>
         <v>1</v>
@@ -22110,7 +21964,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E56">
         <f t="shared" ref="E56:O56" si="15">IF(E17&gt;0,E38/E17,"")</f>
         <v>1</v>
@@ -22156,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D57">
         <f t="shared" ref="D57:O57" si="16">IF(D18&gt;0,D39/D18,"")</f>
         <v>1</v>
@@ -22206,7 +22060,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C58">
         <f t="shared" ref="C58:O58" si="17">IF(C19&gt;0,C40/C19,"")</f>
         <v>1</v>
@@ -22260,7 +22114,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C59" t="str">
         <f t="shared" ref="C59:O60" si="18">IF(C41&gt;0,C20/C41,"")</f>
         <v/>
@@ -22314,7 +22168,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C60" t="str">
         <f t="shared" si="18"/>
         <v/>

</xml_diff>